<commit_message>
template fix + qty numeric
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/sell/template.xlsx
+++ b/src/main/resources/templates/sell/template.xlsx
@@ -8,7 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Inventory" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Attachments" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">Inventory.Sku.Item.Name</t>
   </si>
@@ -28,6 +29,9 @@
     <t xml:space="preserve">Inventory.Sku.PackagingUOM.Name</t>
   </si>
   <si>
+    <t xml:space="preserve">Inventory.Sku.Name</t>
+  </si>
+  <si>
     <t xml:space="preserve">Inventory.Sku.Item.AssetCode.Code</t>
   </si>
   <si>
@@ -47,16 +51,38 @@
   </si>
   <si>
     <t xml:space="preserve">Inventory.Infinite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inventory.Sku.AttachmentUrl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UploadUrl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sku.Item.Company.Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sku.Item.Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sku.PackagingUOM.Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sku.PackagingUOM.Measures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sku.Company.Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -78,13 +104,25 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CCFF"/>
+        <bgColor rgb="FF33CCCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -121,13 +159,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -147,52 +197,61 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="73.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="58.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="31.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="26.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="92.58"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="12" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -204,4 +263,54 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="92.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="73.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="31.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.81"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>